<commit_message>
Fix category case sensitivity issue - normalize default category to match ML model output
Co-authored-by: vamshi620 <27879038+vamshi620@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/test_output/Update_Records.xlsx
+++ b/test_output/Update_Records.xlsx
@@ -44,6 +44,24 @@
   </x:si>
   <x:si>
     <x:t>Update</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alice Brown</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alice@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marketing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Charlie Wilson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>charlie@example.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sales</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -409,14 +427,14 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E2"/>
+  <x:dimension ref="A1:E4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="10.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="18.853482" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="13.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="20.710625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="11.710625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="25.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="18.139196" style="0" customWidth="1"/>
@@ -453,6 +471,34 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>

</xml_diff>